<commit_message>
Implement Fruit and Benchmark Plots
</commit_message>
<xml_diff>
--- a/backend/data/Datenarten_BP6_6_Berechnung5 neueWerte.xlsx
+++ b/backend/data/Datenarten_BP6_6_Berechnung5 neueWerte.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AdrianWild\Dev\Benchmark\backend\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65F4F708-E2E9-44F8-AAEC-C1DB85AEDED0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2B29E3D-0D4F-4E7A-90F9-66623CDB3487}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Basis" sheetId="1" r:id="rId1"/>
@@ -3447,7 +3447,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3532,6 +3532,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -3577,7 +3583,7 @@
     <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3674,6 +3680,8 @@
     <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Komma" xfId="1" builtinId="3"/>
@@ -15176,8 +15184,8 @@
   </sheetPr>
   <dimension ref="A1:H308"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C135" sqref="C135"/>
+    <sheetView tabSelected="1" topLeftCell="A139" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C157" sqref="C157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16731,7 +16739,7 @@
       <c r="B157" t="s">
         <v>693</v>
       </c>
-      <c r="C157">
+      <c r="C157" s="66">
         <v>1</v>
       </c>
       <c r="D157" t="s">
@@ -16742,7 +16750,7 @@
       <c r="B158" t="s">
         <v>694</v>
       </c>
-      <c r="C158">
+      <c r="C158" s="67">
         <v>10</v>
       </c>
       <c r="D158" s="39" t="s">
@@ -18790,8 +18798,8 @@
   </sheetPr>
   <dimension ref="A1:O316"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K90" sqref="K90"/>
+    <sheetView topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M56" sqref="M56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>